<commit_message>
Admin and Development Work
</commit_message>
<xml_diff>
--- a/Z.Assets/SamsaraExcel.xlsx
+++ b/Z.Assets/SamsaraExcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Drive\Writing Grand Compile\Repository\Project Samsara\Obsidian\ProjectSamsara\3. Scribbling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Drive\Writing Grand Compile\Repository\Project Samsara\Obsidian\ProjectSamsara\Z.Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0130B884-5076-4342-9D56-0BB2DE9D8F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B5B57B-5172-43CB-B1C4-5DAB5213DECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="300" windowWidth="23256" windowHeight="12804" tabRatio="790" activeTab="2" xr2:uid="{E6D84C89-D0D8-4C46-AF33-8B126112E9FD}"/>
   </bookViews>
@@ -4621,10 +4621,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -20144,7 +20144,7 @@
   <dimension ref="A1:AD23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+      <selection activeCell="X24" sqref="X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24983,7 +24983,7 @@
       <c r="E4" s="72" t="s">
         <v>317</v>
       </c>
-      <c r="F4" s="322"/>
+      <c r="F4" s="321"/>
       <c r="G4" s="67">
         <v>30</v>
       </c>
@@ -25019,7 +25019,7 @@
       <c r="E5" s="72" t="s">
         <v>317</v>
       </c>
-      <c r="F5" s="322"/>
+      <c r="F5" s="321"/>
       <c r="G5" s="67">
         <v>20</v>
       </c>
@@ -25055,7 +25055,7 @@
       <c r="E6" s="72" t="s">
         <v>318</v>
       </c>
-      <c r="F6" s="322"/>
+      <c r="F6" s="321"/>
       <c r="G6" s="67">
         <v>10</v>
       </c>
@@ -25091,7 +25091,7 @@
       <c r="E7" s="72" t="s">
         <v>319</v>
       </c>
-      <c r="F7" s="321"/>
+      <c r="F7" s="322"/>
       <c r="G7" s="67">
         <v>5</v>
       </c>
@@ -25165,7 +25165,7 @@
       <c r="E9" s="74" t="s">
         <v>319</v>
       </c>
-      <c r="F9" s="322"/>
+      <c r="F9" s="321"/>
       <c r="G9" s="67">
         <v>40</v>
       </c>
@@ -25201,7 +25201,7 @@
       <c r="E10" s="75" t="s">
         <v>320</v>
       </c>
-      <c r="F10" s="321"/>
+      <c r="F10" s="322"/>
       <c r="G10" s="68">
         <v>20</v>
       </c>
@@ -25289,7 +25289,7 @@
       <c r="E13" s="77" t="s">
         <v>317</v>
       </c>
-      <c r="F13" s="322"/>
+      <c r="F13" s="321"/>
       <c r="G13" s="67">
         <v>20</v>
       </c>
@@ -25325,7 +25325,7 @@
       <c r="E14" s="77" t="s">
         <v>317</v>
       </c>
-      <c r="F14" s="322"/>
+      <c r="F14" s="321"/>
       <c r="G14" s="67">
         <v>25</v>
       </c>
@@ -25361,7 +25361,7 @@
       <c r="E15" s="77" t="s">
         <v>318</v>
       </c>
-      <c r="F15" s="322"/>
+      <c r="F15" s="321"/>
       <c r="G15" s="67">
         <v>15</v>
       </c>
@@ -25397,7 +25397,7 @@
       <c r="E16" s="77" t="s">
         <v>318</v>
       </c>
-      <c r="F16" s="322"/>
+      <c r="F16" s="321"/>
       <c r="G16" s="67">
         <v>10</v>
       </c>
@@ -25433,7 +25433,7 @@
       <c r="E17" s="77" t="s">
         <v>319</v>
       </c>
-      <c r="F17" s="321"/>
+      <c r="F17" s="322"/>
       <c r="G17" s="67">
         <v>5</v>
       </c>
@@ -25507,7 +25507,7 @@
       <c r="E19" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="F19" s="322"/>
+      <c r="F19" s="321"/>
       <c r="G19" s="67">
         <v>20</v>
       </c>
@@ -25543,7 +25543,7 @@
       <c r="E20" s="80" t="s">
         <v>320</v>
       </c>
-      <c r="F20" s="321"/>
+      <c r="F20" s="322"/>
       <c r="G20" s="68">
         <v>10</v>
       </c>
@@ -25631,7 +25631,7 @@
       <c r="E23" s="82" t="s">
         <v>317</v>
       </c>
-      <c r="F23" s="322"/>
+      <c r="F23" s="321"/>
       <c r="G23" s="67">
         <v>60</v>
       </c>
@@ -25667,7 +25667,7 @@
       <c r="E24" s="82" t="s">
         <v>317</v>
       </c>
-      <c r="F24" s="322"/>
+      <c r="F24" s="321"/>
       <c r="G24" s="67">
         <v>15</v>
       </c>
@@ -25703,7 +25703,7 @@
       <c r="E25" s="82" t="s">
         <v>317</v>
       </c>
-      <c r="F25" s="322"/>
+      <c r="F25" s="321"/>
       <c r="G25" s="67">
         <v>5</v>
       </c>
@@ -25777,7 +25777,7 @@
       <c r="E27" s="83" t="s">
         <v>319</v>
       </c>
-      <c r="F27" s="322"/>
+      <c r="F27" s="321"/>
       <c r="G27" s="67">
         <v>50</v>
       </c>
@@ -25813,7 +25813,7 @@
       <c r="E28" s="84" t="s">
         <v>319</v>
       </c>
-      <c r="F28" s="321"/>
+      <c r="F28" s="322"/>
       <c r="G28" s="68">
         <v>20</v>
       </c>
@@ -25901,7 +25901,7 @@
       <c r="E31" s="86" t="s">
         <v>318</v>
       </c>
-      <c r="F31" s="322"/>
+      <c r="F31" s="321"/>
       <c r="G31" s="67">
         <v>60</v>
       </c>
@@ -25937,7 +25937,7 @@
       <c r="E32" s="86" t="s">
         <v>318</v>
       </c>
-      <c r="F32" s="322"/>
+      <c r="F32" s="321"/>
       <c r="G32" s="67">
         <v>15</v>
       </c>
@@ -25973,7 +25973,7 @@
       <c r="E33" s="86" t="s">
         <v>319</v>
       </c>
-      <c r="F33" s="322"/>
+      <c r="F33" s="321"/>
       <c r="G33" s="67">
         <v>10</v>
       </c>
@@ -26009,7 +26009,7 @@
       <c r="E34" s="86" t="s">
         <v>319</v>
       </c>
-      <c r="F34" s="322"/>
+      <c r="F34" s="321"/>
       <c r="G34" s="67">
         <v>5</v>
       </c>
@@ -26083,7 +26083,7 @@
       <c r="E36" s="87" t="s">
         <v>319</v>
       </c>
-      <c r="F36" s="322"/>
+      <c r="F36" s="321"/>
       <c r="G36" s="67">
         <v>70</v>
       </c>
@@ -26119,7 +26119,7 @@
       <c r="E37" s="88" t="s">
         <v>320</v>
       </c>
-      <c r="F37" s="321"/>
+      <c r="F37" s="322"/>
       <c r="G37" s="68">
         <v>10</v>
       </c>
@@ -26207,7 +26207,7 @@
       <c r="E40" s="90" t="s">
         <v>317</v>
       </c>
-      <c r="F40" s="322"/>
+      <c r="F40" s="321"/>
       <c r="G40" s="67">
         <v>50</v>
       </c>
@@ -26243,7 +26243,7 @@
       <c r="E41" s="90" t="s">
         <v>317</v>
       </c>
-      <c r="F41" s="322"/>
+      <c r="F41" s="321"/>
       <c r="G41" s="67">
         <v>20</v>
       </c>
@@ -26279,7 +26279,7 @@
       <c r="E42" s="90" t="s">
         <v>318</v>
       </c>
-      <c r="F42" s="322"/>
+      <c r="F42" s="321"/>
       <c r="G42" s="67">
         <v>10</v>
       </c>
@@ -26353,7 +26353,7 @@
       <c r="E44" s="91" t="s">
         <v>318</v>
       </c>
-      <c r="F44" s="322"/>
+      <c r="F44" s="321"/>
       <c r="G44" s="67">
         <v>10</v>
       </c>
@@ -26389,7 +26389,7 @@
       <c r="E45" s="91" t="s">
         <v>319</v>
       </c>
-      <c r="F45" s="322"/>
+      <c r="F45" s="321"/>
       <c r="G45" s="67">
         <v>30</v>
       </c>
@@ -26425,7 +26425,7 @@
       <c r="E46" s="92" t="s">
         <v>320</v>
       </c>
-      <c r="F46" s="321"/>
+      <c r="F46" s="322"/>
       <c r="G46" s="68">
         <v>10</v>
       </c>
@@ -26513,7 +26513,7 @@
       <c r="E49" s="94" t="s">
         <v>318</v>
       </c>
-      <c r="F49" s="322"/>
+      <c r="F49" s="321"/>
       <c r="G49" s="67">
         <v>20</v>
       </c>
@@ -26549,7 +26549,7 @@
       <c r="E50" s="94" t="s">
         <v>318</v>
       </c>
-      <c r="F50" s="322"/>
+      <c r="F50" s="321"/>
       <c r="G50" s="67">
         <v>10</v>
       </c>
@@ -26675,7 +26675,7 @@
       <c r="E54" s="96" t="s">
         <v>317</v>
       </c>
-      <c r="F54" s="322"/>
+      <c r="F54" s="321"/>
       <c r="G54" s="67">
         <v>20</v>
       </c>
@@ -26711,7 +26711,7 @@
       <c r="E55" s="96" t="s">
         <v>318</v>
       </c>
-      <c r="F55" s="322"/>
+      <c r="F55" s="321"/>
       <c r="G55" s="67">
         <v>10</v>
       </c>
@@ -26785,7 +26785,7 @@
       <c r="E57" s="97" t="s">
         <v>319</v>
       </c>
-      <c r="F57" s="322"/>
+      <c r="F57" s="321"/>
       <c r="G57" s="67">
         <v>15</v>
       </c>
@@ -26821,7 +26821,7 @@
       <c r="E58" s="98" t="s">
         <v>319</v>
       </c>
-      <c r="F58" s="321"/>
+      <c r="F58" s="322"/>
       <c r="G58" s="68">
         <v>5</v>
       </c>
@@ -26909,7 +26909,7 @@
       <c r="E61" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="F61" s="322"/>
+      <c r="F61" s="321"/>
       <c r="G61" s="67">
         <v>20</v>
       </c>
@@ -26945,7 +26945,7 @@
       <c r="E62" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="F62" s="322"/>
+      <c r="F62" s="321"/>
       <c r="G62" s="67">
         <v>20</v>
       </c>
@@ -26981,7 +26981,7 @@
       <c r="E63" s="100" t="s">
         <v>320</v>
       </c>
-      <c r="F63" s="322"/>
+      <c r="F63" s="321"/>
       <c r="G63" s="67">
         <v>15</v>
       </c>
@@ -27017,7 +27017,7 @@
       <c r="E64" s="100" t="s">
         <v>320</v>
       </c>
-      <c r="F64" s="322"/>
+      <c r="F64" s="321"/>
       <c r="G64" s="67">
         <v>15</v>
       </c>
@@ -27053,7 +27053,7 @@
       <c r="E65" s="100" t="s">
         <v>320</v>
       </c>
-      <c r="F65" s="322"/>
+      <c r="F65" s="321"/>
       <c r="G65" s="67">
         <v>10</v>
       </c>
@@ -27127,7 +27127,7 @@
       <c r="E67" s="101" t="s">
         <v>321</v>
       </c>
-      <c r="F67" s="321"/>
+      <c r="F67" s="322"/>
       <c r="G67" s="68">
         <v>20</v>
       </c>
@@ -27215,7 +27215,7 @@
       <c r="E70" s="103" t="s">
         <v>318</v>
       </c>
-      <c r="F70" s="322"/>
+      <c r="F70" s="321"/>
       <c r="G70" s="67">
         <v>35</v>
       </c>
@@ -27251,7 +27251,7 @@
       <c r="E71" s="103" t="s">
         <v>318</v>
       </c>
-      <c r="F71" s="322"/>
+      <c r="F71" s="321"/>
       <c r="G71" s="67">
         <v>20</v>
       </c>
@@ -27287,7 +27287,7 @@
       <c r="E72" s="103" t="s">
         <v>319</v>
       </c>
-      <c r="F72" s="322"/>
+      <c r="F72" s="321"/>
       <c r="G72" s="67">
         <v>10</v>
       </c>
@@ -27361,7 +27361,7 @@
       <c r="E74" s="104" t="s">
         <v>320</v>
       </c>
-      <c r="F74" s="321"/>
+      <c r="F74" s="322"/>
       <c r="G74" s="68">
         <v>75</v>
       </c>
@@ -27411,7 +27411,7 @@
       <c r="E76" s="105" t="s">
         <v>320</v>
       </c>
-      <c r="F76" s="322">
+      <c r="F76" s="321">
         <v>60</v>
       </c>
       <c r="G76" s="67">
@@ -27449,7 +27449,7 @@
       <c r="E77" s="105" t="s">
         <v>320</v>
       </c>
-      <c r="F77" s="322"/>
+      <c r="F77" s="321"/>
       <c r="G77" s="67">
         <v>75</v>
       </c>
@@ -27523,7 +27523,7 @@
       <c r="E79" s="106" t="s">
         <v>321</v>
       </c>
-      <c r="F79" s="321"/>
+      <c r="F79" s="322"/>
       <c r="G79" s="68">
         <v>75</v>
       </c>
@@ -27658,6 +27658,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="F76:F77"/>
+    <mergeCell ref="F78:F79"/>
+    <mergeCell ref="F48:F50"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F60:F65"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="F69:F72"/>
     <mergeCell ref="F43:F46"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:L1"/>
@@ -27670,15 +27679,6 @@
     <mergeCell ref="F30:F34"/>
     <mergeCell ref="F35:F37"/>
     <mergeCell ref="F39:F42"/>
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="F76:F77"/>
-    <mergeCell ref="F78:F79"/>
-    <mergeCell ref="F48:F50"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F60:F65"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="F69:F72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>